<commit_message>
update banyak add moble eyevent
</commit_message>
<xml_diff>
--- a/Dokumen/iklan.xlsx
+++ b/Dokumen/iklan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="112">
   <si>
     <t>Nama Iklan</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Home Page Banner Ads</t>
   </si>
   <si>
-    <t>Ads Jumbo</t>
-  </si>
-  <si>
     <t>1065 x 300</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Full Width Ads</t>
   </si>
   <si>
-    <t>1065 x 100</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
     <t>Diatas Konten Rekomendasi</t>
   </si>
   <si>
-    <t>690 x 100</t>
-  </si>
-  <si>
     <t>Diatas Komentar</t>
   </si>
   <si>
@@ -237,6 +228,141 @@
   </si>
   <si>
     <t>AD Space Versi Web Mobile</t>
+  </si>
+  <si>
+    <t>Nama File</t>
+  </si>
+  <si>
+    <t>Kode Iklan</t>
+  </si>
+  <si>
+    <t>HOME.png</t>
+  </si>
+  <si>
+    <t>#A1</t>
+  </si>
+  <si>
+    <t>#HOME1</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub-ofisial-detail.png</t>
+  </si>
+  <si>
+    <t>#EyeProfile1</t>
+  </si>
+  <si>
+    <t>#EyeProfile2</t>
+  </si>
+  <si>
+    <t>#EyeProfile3</t>
+  </si>
+  <si>
+    <t>#EyeProfile4</t>
+  </si>
+  <si>
+    <t>#EyeProfile5</t>
+  </si>
+  <si>
+    <t>#EyeProfile6</t>
+  </si>
+  <si>
+    <t>#EyeProfile7</t>
+  </si>
+  <si>
+    <t>#EyeProfile8</t>
+  </si>
+  <si>
+    <t>#EyeProfile9</t>
+  </si>
+  <si>
+    <t>#EyeProfile10</t>
+  </si>
+  <si>
+    <t>#EyeProfile11</t>
+  </si>
+  <si>
+    <t>#EyeProfile12</t>
+  </si>
+  <si>
+    <t>#EyeProfile13</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub-ofisial.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub-pemain-detail.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub-pemain.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub-suporter.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-klub.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-liga-klub.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-liga-suporter-detail.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-liga-suporter.png</t>
+  </si>
+  <si>
+    <t>eyeprofile-liga.png</t>
+  </si>
+  <si>
+    <t>eyenews-detail.png</t>
+  </si>
+  <si>
+    <t>#EyeNews1</t>
+  </si>
+  <si>
+    <t>#EyeNews2</t>
+  </si>
+  <si>
+    <t>#EyeNews3</t>
+  </si>
+  <si>
+    <t>#EyeNews4</t>
+  </si>
+  <si>
+    <t>1065 x 120</t>
+  </si>
+  <si>
+    <t>690 x 120</t>
+  </si>
+  <si>
+    <t>425 x 120</t>
+  </si>
+  <si>
+    <t>eyenews-kategori.png</t>
+  </si>
+  <si>
+    <t>eyenews.png</t>
+  </si>
+  <si>
+    <t>eyetube-detail.png</t>
+  </si>
+  <si>
+    <t>eyetube.png</t>
+  </si>
+  <si>
+    <t>#EyeTube1</t>
+  </si>
+  <si>
+    <t>#EyeTube2</t>
+  </si>
+  <si>
+    <t>#EyeTube3</t>
+  </si>
+  <si>
+    <t>#EyeVent1</t>
+  </si>
+  <si>
+    <t>eyevent-detail.png</t>
   </si>
 </sst>
 </file>
@@ -305,27 +431,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F32"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,11 +749,13 @@
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="73.83203125" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
+    <row r="1" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -627,9 +763,9 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -641,23 +777,29 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -671,13 +813,19 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -685,481 +833,613 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
       <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+      <c r="D8" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
       <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
+      <c r="D14" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
       <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>19</v>
       </c>
       <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
       <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="G27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
         <v>14</v>
       </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="G28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
       <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
         <v>10</v>
       </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="G30" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>

</xml_diff>